<commit_message>
readme file draft creation
</commit_message>
<xml_diff>
--- a/Design/User Stories/UserStories.xlsx
+++ b/Design/User Stories/UserStories.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aninditasom/Desktop/Code Institute Project/MS4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aninditasom/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD50E90F-FA28-1C42-BC30-FFE83D6F5829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41921F8-15A3-024A-AD23-332881EFBB78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="960" windowWidth="27360" windowHeight="16540" xr2:uid="{722DA055-67F5-1249-A473-6E5F737A2630}"/>
+    <workbookView xWindow="1080" yWindow="960" windowWidth="27340" windowHeight="16540" xr2:uid="{3A95C946-8E90-AE4B-AEB2-2E761B2BB9A0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="User Stories" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$D$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories'!$A$1:$D$29</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t>User Story ID</t>
   </si>
@@ -213,12 +213,6 @@
     <t>use the mail for a formal confirmation of the items that has been purchased</t>
   </si>
   <si>
-    <t>send any workshop as a gift by providing a different shipping address</t>
-  </si>
-  <si>
-    <t>Invite a friend to the workshop</t>
-  </si>
-  <si>
     <t>Blogs and User Comments</t>
   </si>
   <si>
@@ -273,7 +267,7 @@
     <t>Add workshops to the database</t>
   </si>
   <si>
-    <t>Notified of any invalid entries for creating a workshop. All workshops should be created for future days</t>
+    <t xml:space="preserve">Notified of any invalid entries for creating a workshop. </t>
   </si>
   <si>
     <t>Make the necessary changes before commiting the records in the database</t>
@@ -337,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -345,17 +339,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -363,8 +455,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,19 +787,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403E0D63-5643-D74C-84F0-84FCC553A42F}">
-  <dimension ref="A1:D43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC852E44-3974-0C40-85CB-33F789F3F9A5}">
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="74" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -699,13 +807,13 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -713,77 +821,77 @@
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -791,63 +899,63 @@
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="8">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="8">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="8">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="8">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -855,49 +963,49 @@
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="8">
         <v>10</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="8">
         <v>11</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16" s="8">
         <v>12</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -905,370 +1013,356 @@
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18" s="8">
         <v>13</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="A19" s="8">
         <v>14</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="A20" s="8">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="A21" s="8">
         <v>16</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="A22" s="8">
         <v>17</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="A23" s="8">
         <v>18</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="A24" s="8">
         <v>19</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="A25" s="8">
         <v>20</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="A26" s="8">
         <v>21</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="A27" s="8">
         <v>22</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="A28" s="8">
         <v>23</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="A29" s="8">
         <v>24</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
         <v>25</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="B31" s="9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="C31" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="D31" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
         <v>26</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
         <v>27</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="C33" s="10" t="s">
         <v>66</v>
       </c>
+      <c r="D33" s="12" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="A34" s="8">
         <v>28</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="A35" s="8">
         <v>29</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="8">
         <v>30</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
         <v>31</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="3" t="s">
+      <c r="B38" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="D38" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+    </row>
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
         <v>32</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B39" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="8">
         <v>33</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B40" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
         <v>34</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="B41" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+    <row r="42" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
         <v>35</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B42" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="17" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
-        <v>36</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A38:D38"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>